<commit_message>
pushed detailed sex correction data
</commit_message>
<xml_diff>
--- a/outputs/R_OUT - Nitinat sex correction 2023.xlsx
+++ b/outputs/R_OUT - Nitinat sex correction 2023.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,80 +370,85 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>TermRun_AGES_year</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>n_sample</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>propn_age_sample</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>n_age_jackCORR</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>n_sample_jackCORR</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>propn_age_sample_jackCORR</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>escapement_estimate</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>true_sex_ratio</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>n_sex_CORR</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>n_sexAge_CORR</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>propn_sexAge_CORR</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>TermRun_AGEStemp</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>TermRun_AGESspat</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>TermRun_AGESsex</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>fecundity</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>total_fecundity</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>total_egg_deposition</t>
         </is>
@@ -458,37 +463,37 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D2">
         <v>221</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I2">
+        <v>14250</v>
+      </c>
+      <c r="J2">
         <v>0.43613707165109</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>6214.953271028033</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M2">
+        <v>0</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -497,16 +502,21 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Female</t>
         </is>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>0</v>
       </c>
     </row>
@@ -519,41 +529,41 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D3">
         <v>221</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.02262443438914027</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>221</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.02262443438914027</v>
       </c>
-      <c r="H3">
-        <v>14250</v>
-      </c>
       <c r="I3">
+        <v>14250</v>
+      </c>
+      <c r="J3">
         <v>0.43613707165109</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6214.953271028033</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>140.6098025119464</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.009867354562241856</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N3" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -561,18 +571,23 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Female</t>
         </is>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>3000</v>
-      </c>
-      <c r="Q3">
-        <v>421829.4075358393</v>
       </c>
       <c r="R3">
         <v>421829.4075358393</v>
       </c>
+      <c r="S3">
+        <v>421829.4075358393</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -583,41 +598,41 @@
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D4">
         <v>221</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.8914027149321267</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>197</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>221</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.8914027149321267</v>
       </c>
-      <c r="H4">
-        <v>14250</v>
-      </c>
       <c r="I4">
+        <v>14250</v>
+      </c>
+      <c r="J4">
         <v>0.43613707165109</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>6214.953271028033</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>5540.02621897069</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.3887737697523291</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -625,18 +640,23 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Female</t>
         </is>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>3500</v>
-      </c>
-      <c r="Q4">
-        <v>19390091.76639742</v>
       </c>
       <c r="R4">
         <v>19390091.76639742</v>
       </c>
+      <c r="S4">
+        <v>19390091.76639742</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -647,41 +667,41 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D5">
         <v>221</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.08144796380090498</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>18</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>221</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.08144796380090498</v>
       </c>
-      <c r="H5">
-        <v>14250</v>
-      </c>
       <c r="I5">
+        <v>14250</v>
+      </c>
+      <c r="J5">
         <v>0.43613707165109</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>6214.953271028033</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>506.1952890430072</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.03552247642407069</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N5" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -689,18 +709,23 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Female</t>
         </is>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>4000</v>
-      </c>
-      <c r="Q5">
-        <v>2024781.156172029</v>
       </c>
       <c r="R5">
         <v>2024781.156172029</v>
       </c>
+      <c r="S5">
+        <v>2024781.156172029</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -711,41 +736,41 @@
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D6">
         <v>221</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.004524886877828055</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>221</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.004524886877828055</v>
       </c>
-      <c r="H6">
-        <v>14250</v>
-      </c>
       <c r="I6">
+        <v>14250</v>
+      </c>
+      <c r="J6">
         <v>0.43613707165109</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>6214.953271028033</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>28.12196050238929</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>0.001973470912448371</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -753,18 +778,23 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Female</t>
         </is>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>4000</v>
-      </c>
-      <c r="Q6">
-        <v>112487.8420095572</v>
       </c>
       <c r="R6">
         <v>112487.8420095572</v>
       </c>
+      <c r="S6">
+        <v>112487.8420095572</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -775,41 +805,41 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D7">
         <v>55</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.7818181818181819</v>
-      </c>
-      <c r="E7">
-        <v>43</v>
       </c>
       <c r="F7">
         <v>43</v>
       </c>
       <c r="G7">
+        <v>43</v>
+      </c>
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="H7">
-        <v>14250</v>
-      </c>
       <c r="I7">
+        <v>14250</v>
+      </c>
+      <c r="J7">
         <v>0.01179328951094816</v>
-      </c>
-      <c r="J7">
-        <v>168.0543755310113</v>
       </c>
       <c r="K7">
         <v>168.0543755310113</v>
       </c>
       <c r="L7">
+        <v>168.0543755310113</v>
+      </c>
+      <c r="M7">
         <v>0.01179328951094816</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N7" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -817,10 +847,15 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>0</v>
       </c>
     </row>
@@ -833,40 +868,40 @@
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D8">
         <v>55</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.1818181818181818</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>43</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I8">
+        <v>14250</v>
+      </c>
+      <c r="J8">
         <v>0.01179328951094816</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>168.0543755310113</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M8">
+        <v>0</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -875,10 +910,15 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>421829.4075358393</v>
       </c>
     </row>
@@ -891,40 +931,40 @@
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D9">
         <v>55</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.03636363636363636</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>43</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I9">
+        <v>14250</v>
+      </c>
+      <c r="J9">
         <v>0.01179328951094816</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>168.0543755310113</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M9">
+        <v>0</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -933,10 +973,15 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>19390091.76639742</v>
       </c>
     </row>
@@ -949,37 +994,37 @@
       <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D10">
         <v>55</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="G10">
+      <c r="F10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I10">
+        <v>14250</v>
+      </c>
+      <c r="J10">
         <v>0.01179328951094816</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>168.0543755310113</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M10">
+        <v>0</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -988,10 +1033,15 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>2024781.156172029</v>
       </c>
     </row>
@@ -1004,37 +1054,37 @@
       <c r="B11">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D11">
         <v>55</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I11">
+        <v>14250</v>
+      </c>
+      <c r="J11">
         <v>0.01179328951094816</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>168.0543755310113</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M11">
+        <v>0</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1043,10 +1093,15 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>112487.8420095572</v>
       </c>
     </row>
@@ -1059,37 +1114,37 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D12">
         <v>333</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I12">
+        <v>14250</v>
+      </c>
+      <c r="J12">
         <v>0.5520696388379619</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>7866.992353440957</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M12">
+        <v>0</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1098,10 +1153,15 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>0</v>
       </c>
     </row>
@@ -1114,41 +1174,41 @@
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D13">
         <v>333</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.1741741741741742</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>68</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>345</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.1971014492753623</v>
       </c>
-      <c r="H13">
-        <v>14250</v>
-      </c>
       <c r="I13">
+        <v>14250</v>
+      </c>
+      <c r="J13">
         <v>0.5520696388379619</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>7866.992353440957</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>1550.595594301406</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.1088137259158882</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N13" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1156,10 +1216,15 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>421829.4075358393</v>
       </c>
     </row>
@@ -1172,41 +1237,41 @@
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D14">
         <v>333</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.8048048048048048</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>270</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>345</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H14">
-        <v>14250</v>
-      </c>
       <c r="I14">
+        <v>14250</v>
+      </c>
+      <c r="J14">
         <v>0.5520696388379619</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>7866.992353440957</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>6156.776624432054</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>0.4320544999601441</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N14" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1214,10 +1279,15 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>19390091.76639742</v>
       </c>
     </row>
@@ -1230,41 +1300,41 @@
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D15">
         <v>333</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.02102102102102102</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>7</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>345</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.02028985507246377</v>
       </c>
-      <c r="H15">
-        <v>14250</v>
-      </c>
       <c r="I15">
+        <v>14250</v>
+      </c>
+      <c r="J15">
         <v>0.5520696388379619</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>7866.992353440957</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>159.6201347074977</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>0.01120141296192966</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N15" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1272,10 +1342,15 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>2024781.156172029</v>
       </c>
     </row>
@@ -1288,37 +1363,37 @@
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D16">
         <v>333</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
       <c r="E16">
         <v>0</v>
       </c>
-      <c r="G16">
+      <c r="F16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>14250</v>
+        <v>0</v>
       </c>
       <c r="I16">
+        <v>14250</v>
+      </c>
+      <c r="J16">
         <v>0.5520696388379619</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>7866.992353440957</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M16">
+        <v>0</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1327,10 +1402,15 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>112487.8420095572</v>
       </c>
     </row>
@@ -1343,23 +1423,23 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D17">
         <v>609</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.07060755336617405</v>
       </c>
-      <c r="H17">
-        <v>14250</v>
-      </c>
-      <c r="L17">
+      <c r="I17">
+        <v>14250</v>
+      </c>
+      <c r="M17">
         <v>0.01179328951094816</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N17" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1367,10 +1447,15 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>0</v>
       </c>
     </row>
@@ -1383,23 +1468,23 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D18">
         <v>609</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.1198686371100164</v>
       </c>
-      <c r="H18">
-        <v>14250</v>
-      </c>
-      <c r="L18">
+      <c r="I18">
+        <v>14250</v>
+      </c>
+      <c r="M18">
         <v>0.11868108047813</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N18" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1407,10 +1492,15 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>421829.4075358393</v>
       </c>
     </row>
@@ -1423,23 +1513,23 @@
       <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D19">
         <v>609</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.7668308702791461</v>
       </c>
-      <c r="H19">
-        <v>14250</v>
-      </c>
-      <c r="L19">
+      <c r="I19">
+        <v>14250</v>
+      </c>
+      <c r="M19">
         <v>0.8208282697124732</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N19" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1447,10 +1537,15 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>19390091.76639742</v>
       </c>
     </row>
@@ -1463,23 +1558,23 @@
       <c r="B20">
         <v>5</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D20">
         <v>609</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0.04105090311986864</v>
       </c>
-      <c r="H20">
-        <v>14250</v>
-      </c>
-      <c r="L20">
+      <c r="I20">
+        <v>14250</v>
+      </c>
+      <c r="M20">
         <v>0.04672388938600035</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N20" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1487,10 +1582,15 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>2024781.156172029</v>
       </c>
     </row>
@@ -1503,23 +1603,23 @@
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D21">
         <v>609</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0.001642036124794745</v>
       </c>
-      <c r="H21">
-        <v>14250</v>
-      </c>
-      <c r="L21">
+      <c r="I21">
+        <v>14250</v>
+      </c>
+      <c r="M21">
         <v>0.001973470912448371</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N21" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1527,10 +1627,15 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>112487.8420095572</v>
       </c>
     </row>
@@ -1543,26 +1648,26 @@
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D22">
         <v>388</v>
       </c>
-      <c r="H22">
-        <v>14250</v>
-      </c>
-      <c r="J22">
+      <c r="I22">
+        <v>14250</v>
+      </c>
+      <c r="K22">
         <v>8035.046728971969</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>168.0543755310113</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>0.01179328951094816</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N22" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1570,10 +1675,15 @@
       </c>
       <c r="O22" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>0</v>
       </c>
     </row>
@@ -1586,26 +1696,26 @@
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D23">
         <v>388</v>
       </c>
-      <c r="H23">
-        <v>14250</v>
-      </c>
-      <c r="J23">
+      <c r="I23">
+        <v>14250</v>
+      </c>
+      <c r="K23">
         <v>8035.046728971969</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>1550.595594301406</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>0.1088137259158882</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N23" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1613,10 +1723,15 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="R23">
+      <c r="S23">
         <v>421829.4075358393</v>
       </c>
     </row>
@@ -1629,26 +1744,26 @@
       <c r="B24">
         <v>4</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D24">
         <v>388</v>
       </c>
-      <c r="H24">
-        <v>14250</v>
-      </c>
-      <c r="J24">
+      <c r="I24">
+        <v>14250</v>
+      </c>
+      <c r="K24">
         <v>8035.046728971969</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>6156.776624432054</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>0.4320544999601441</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N24" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1656,10 +1771,15 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="R24">
+      <c r="S24">
         <v>19390091.76639742</v>
       </c>
     </row>
@@ -1672,26 +1792,26 @@
       <c r="B25">
         <v>5</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D25">
         <v>388</v>
       </c>
-      <c r="H25">
-        <v>14250</v>
-      </c>
-      <c r="J25">
+      <c r="I25">
+        <v>14250</v>
+      </c>
+      <c r="K25">
         <v>8035.046728971969</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>159.6201347074977</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>0.01120141296192966</v>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
-      </c>
       <c r="N25" t="inlineStr">
         <is>
           <t>Broodstock corrected</t>
@@ -1699,10 +1819,15 @@
       </c>
       <c r="O25" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="R25">
+      <c r="S25">
         <v>2024781.156172029</v>
       </c>
     </row>
@@ -1715,25 +1840,25 @@
       <c r="B26">
         <v>6</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D26">
         <v>388</v>
       </c>
-      <c r="H26">
-        <v>14250</v>
-      </c>
-      <c r="J26">
+      <c r="I26">
+        <v>14250</v>
+      </c>
+      <c r="K26">
         <v>8035.046728971969</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Broodstock corrected</t>
-        </is>
+      <c r="M26">
+        <v>0</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
@@ -1742,10 +1867,15 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
+          <t>Broodstock corrected</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="R26">
+      <c r="S26">
         <v>112487.8420095572</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update outputs from 02
</commit_message>
<xml_diff>
--- a/outputs/R_OUT - Nitinat sex correction 2023.xlsx
+++ b/outputs/R_OUT - Nitinat sex correction 2023.xlsx
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>21949190.17211484</v>
       </c>
     </row>
     <row r="3">
@@ -586,7 +586,7 @@
         <v>421829.4075358393</v>
       </c>
       <c r="S3">
-        <v>421829.4075358393</v>
+        <v>21949190.17211484</v>
       </c>
     </row>
     <row r="4">
@@ -655,7 +655,7 @@
         <v>19390091.76639742</v>
       </c>
       <c r="S4">
-        <v>19390091.76639742</v>
+        <v>21949190.17211484</v>
       </c>
     </row>
     <row r="5">
@@ -724,7 +724,7 @@
         <v>2024781.156172029</v>
       </c>
       <c r="S5">
-        <v>2024781.156172029</v>
+        <v>21949190.17211484</v>
       </c>
     </row>
     <row r="6">
@@ -793,7 +793,7 @@
         <v>112487.8420095572</v>
       </c>
       <c r="S6">
-        <v>112487.8420095572</v>
+        <v>21949190.17211484</v>
       </c>
     </row>
     <row r="7">
@@ -838,7 +838,7 @@
         <v>168.0543755310113</v>
       </c>
       <c r="M7">
-        <v>0.01179328951094816</v>
+        <v>0.7818181818181819</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -854,9 +854,6 @@
         <is>
           <t>Broodstock corrected - Jack</t>
         </is>
-      </c>
-      <c r="S7">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -918,9 +915,6 @@
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="S8">
-        <v>421829.4075358393</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -981,9 +975,6 @@
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="S9">
-        <v>19390091.76639742</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1041,9 +1032,6 @@
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="S10">
-        <v>2024781.156172029</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1101,9 +1089,6 @@
           <t>Broodstock corrected - Jack</t>
         </is>
       </c>
-      <c r="S11">
-        <v>112487.8420095572</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1161,9 +1146,6 @@
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1224,9 +1206,6 @@
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="S13">
-        <v>421829.4075358393</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1287,9 +1266,6 @@
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="S14">
-        <v>19390091.76639742</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1350,9 +1326,6 @@
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="S15">
-        <v>2024781.156172029</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1410,9 +1383,6 @@
           <t>Broodstock corrected - Male</t>
         </is>
       </c>
-      <c r="S16">
-        <v>112487.8420095572</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1455,9 +1425,6 @@
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1500,9 +1467,6 @@
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="S18">
-        <v>421829.4075358393</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1545,9 +1509,6 @@
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="S19">
-        <v>19390091.76639742</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1590,9 +1551,6 @@
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="S20">
-        <v>2024781.156172029</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1635,9 +1593,6 @@
           <t>Broodstock corrected - Total</t>
         </is>
       </c>
-      <c r="S21">
-        <v>112487.8420095572</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1683,9 +1638,6 @@
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1731,9 +1683,6 @@
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="S23">
-        <v>421829.4075358393</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1779,9 +1728,6 @@
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="S24">
-        <v>19390091.76639742</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1827,9 +1773,6 @@
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
       </c>
-      <c r="S25">
-        <v>2024781.156172029</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1874,9 +1817,6 @@
         <is>
           <t>Broodstock corrected - Males (incl Jacks)</t>
         </is>
-      </c>
-      <c r="S26">
-        <v>112487.8420095572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>